<commit_message>
all data cleaned in the new subfolder, only missing thing is futures timeseries for hedge
</commit_message>
<xml_diff>
--- a/Data_Inflation.xlsx
+++ b/Data_Inflation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Library/CloudStorage/Dropbox/00 UZH/Master/PMP/01. Offline PMP/PMP Coding/PMP-Term-Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D03A1A-4617-944A-8406-240933AF7B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA53F71-E6C0-E24D-8EB7-04115452281A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26800" xr2:uid="{5E242D33-EFCD-464F-8E19-878E41535C64}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="54">
   <si>
     <t>Datum</t>
   </si>
@@ -128,12 +128,84 @@
   <si>
     <t>INFUTOTY Index</t>
   </si>
+  <si>
+    <t>Target Rate</t>
+  </si>
+  <si>
+    <t>since 31.12.2003</t>
+  </si>
+  <si>
+    <t>0.02 - 0.06</t>
+  </si>
+  <si>
+    <t>since 31.03.2016</t>
+  </si>
+  <si>
+    <t>since 31.12.2011</t>
+  </si>
+  <si>
+    <t>0.017 - 0.02</t>
+  </si>
+  <si>
+    <t>before 2012</t>
+  </si>
+  <si>
+    <t>since 22.01.2013</t>
+  </si>
+  <si>
+    <t>0.02 - 0.03</t>
+  </si>
+  <si>
+    <t>India: The Reserve Bank of India has changed its target inflation rate over time. From 1998-2015, the target was an inflation rate of 4% with a +/- 2% tolerance range. In 2016, the RBI adopted a new monetary policy framework, and the target was changed to a headline inflation rate of 4% (+/- 2%) until March 2021. In April 2021, the RBI announced a new target range of 2-6% for the next five years.</t>
+  </si>
+  <si>
+    <t>Singapore: The Monetary Authority of Singapore has adopted a policy of targeting medium-term price stability, and does not have a specific numerical target for inflation.</t>
+  </si>
+  <si>
+    <t>Canada: The Bank of Canada has changed its target inflation rate over time. From 1991 to 2001, the target was a range of 1% to 3%. From 2002 to 2011, the target was a 2% inflation rate. In 2012, the Bank of Canada adopted a new policy of targeting a 2% inflation rate that is "flexible" in the short term.</t>
+  </si>
+  <si>
+    <t>USA: The Federal Reserve has changed its target inflation rate over time. From 1996 to 2011, the target was a 2% inflation rate. In August 2020, the Federal Reserve announced a new policy of "average inflation targeting," where it would aim to achieve inflation that averages 2% over time, rather than targeting a specific rate.</t>
+  </si>
+  <si>
+    <t>Japan: The Bank of Japan has had a target inflation rate of 2% since 2013, as part of its "Quantitative and Qualitative Monetary Easing" policy. Prior to that, the Bank of Japan had various inflation targets, including a 1% target from 2010 to 2013.</t>
+  </si>
+  <si>
+    <t>Australia: The Reserve Bank of Australia has changed its target inflation rate over time. From 1993 to 2016, the target was a 2% to 3% inflation rate. In 2016, the target was changed to a 2% inflation rate, with a "flexible medium-term inflation target."</t>
+  </si>
+  <si>
+    <t>China: The People's Bank of China does not have a specific inflation target, but aims for "reasonable and stable" inflation.</t>
+  </si>
+  <si>
+    <t>Switzerland: The Swiss National Bank has had a target inflation rate of below 2% since 2000.</t>
+  </si>
+  <si>
+    <t>UK: The Bank of England has changed its target inflation rate over time. From 1992 to 2003, the target was a 2.5% inflation rate. From 2004 to 2013, the target was a 2% inflation rate. In 2013, the Bank of England adopted a "forward guidance" policy, where it would not consider raising interest rates until the unemployment rate fell below 7%. In 2015, the Bank of England returned to targeting a 2% inflation rate.</t>
+  </si>
+  <si>
+    <t>Spain: The Bank of Spain does not have a specific inflation target, but aims for price stability in the eurozone.</t>
+  </si>
+  <si>
+    <t>France: The Bank of France does not have a specific inflation target, but aims for price stability in the eurozone.</t>
+  </si>
+  <si>
+    <t>Germany: The Bundesbank does not have a specific inflation target, but aims for price stability in the eurozone.</t>
+  </si>
+  <si>
+    <t>Italy: The Bank of Italy does not have a specific inflation target, but aims for price stability in the eurozone.</t>
+  </si>
+  <si>
+    <t>before 31.03.2016</t>
+  </si>
+  <si>
+    <t>"reflects our interpretation of reasonable and stable" inflation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +225,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -181,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -190,6 +269,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -507,7 +587,7 @@
   <dimension ref="A1:N283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12972,12 +13052,237 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6645157-D0A0-0B43-8667-38B453D0762F}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:N34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>0.02</v>
+      </c>
+      <c r="D3">
+        <v>0.02</v>
+      </c>
+      <c r="E3">
+        <v>0.02</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3">
+        <v>0.02</v>
+      </c>
+      <c r="I3">
+        <v>0.02</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="K3">
+        <v>0.02</v>
+      </c>
+      <c r="L3">
+        <v>0.02</v>
+      </c>
+      <c r="M3">
+        <v>0.02</v>
+      </c>
+      <c r="N3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>0.04</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>